<commit_message>
Implemented complete dynamics linearization
</commit_message>
<xml_diff>
--- a/maglev_results.xlsx
+++ b/maglev_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9314afe84198813/Documents/Skool/Semester 9/481 Linear Systems/Labs/Code/Lab_Project_Git/ELEC481/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_B359E617CF19DF9FAD388B0AE0822A6871042643" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C2B1911-44E8-435C-BDBB-748A4919616E}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_B359E617CF19DF5FA93D4FAAE1822A68710448FA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{763954E8-B0F5-4430-9A66-7FAA59547DA4}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-14960" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,25 +418,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
     <col min="2" max="2" width="9.7265625" customWidth="1"/>
     <col min="3" max="6" width="11.453125" customWidth="1"/>
     <col min="7" max="7" width="9.6328125" customWidth="1"/>
-    <col min="8" max="10" width="1.90625" customWidth="1"/>
+    <col min="8" max="8" width="1.90625" customWidth="1"/>
+    <col min="9" max="10" width="15.7265625" customWidth="1"/>
     <col min="11" max="11" width="14.453125" customWidth="1"/>
     <col min="12" max="12" width="9.6328125" customWidth="1"/>
-    <col min="13" max="15" width="1.90625" customWidth="1"/>
+    <col min="13" max="13" width="1.90625" customWidth="1"/>
+    <col min="14" max="15" width="15.7265625" customWidth="1"/>
     <col min="16" max="16" width="14.453125" customWidth="1"/>
-    <col min="17" max="17" width="12.453125" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" customWidth="1"/>
+    <col min="17" max="18" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
@@ -479,16 +480,16 @@
         <v>-0.1</v>
       </c>
       <c r="C2">
-        <v>3796.857583088145</v>
+        <v>4005.9683493065641</v>
       </c>
       <c r="D2">
-        <v>2322.7896943478545</v>
+        <v>2204.8371461562447</v>
       </c>
       <c r="E2">
-        <v>1.9618317492261179</v>
+        <v>3.8041409678215623</v>
       </c>
       <c r="F2">
-        <v>1.9618317492261177</v>
+        <v>2.9861922376603327</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -497,13 +498,13 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>-4.705659626696994E-5</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>-1.1764149066742443E-5</v>
       </c>
       <c r="K2">
-        <v>1.8904238278936779E-3</v>
+        <v>2.5186071013528696E-3</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -512,19 +513,19 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>-4.7056596266969933E-5</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>-1.1764149066742316E-5</v>
       </c>
       <c r="P2">
-        <v>1.8904238278936779E-3</v>
+        <v>1.9267237441451676E-3</v>
       </c>
       <c r="Q2">
-        <v>0.48990925251853246</v>
+        <v>0.55019652757935256</v>
       </c>
       <c r="R2">
-        <v>2.0411943535648405</v>
+        <v>1.8175323722954142</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -535,16 +536,16 @@
         <v>-0.2</v>
       </c>
       <c r="C3">
-        <v>4084.1560682530371</v>
+        <v>4318.9229147504038</v>
       </c>
       <c r="D3">
-        <v>2433.389694562964</v>
+        <v>2304.4777323350422</v>
       </c>
       <c r="E3">
-        <v>2.0466219755768309</v>
+        <v>4.0128383554782312</v>
       </c>
       <c r="F3">
-        <v>2.0466219755768309</v>
+        <v>3.1519516220210639</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -553,13 +554,13 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>-4.811104491031333E-5</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>-1.2027761227578248E-5</v>
       </c>
       <c r="K3">
-        <v>1.8900118280221834E-3</v>
+        <v>2.512186949154884E-3</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -568,19 +569,19 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>-4.811104491031333E-5</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>-1.2027761227578461E-5</v>
       </c>
       <c r="P3">
-        <v>1.8900118280221834E-3</v>
+        <v>1.9160502731082887E-3</v>
       </c>
       <c r="Q3">
-        <v>0.50109448799856693</v>
+        <v>0.56628067135680671</v>
       </c>
       <c r="R3">
-        <v>1.9956316103059188</v>
+        <v>1.7659087632357346</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -591,16 +592,16 @@
         <v>-0.30000000000000004</v>
       </c>
       <c r="C4">
-        <v>4391.2801767345118</v>
+        <v>4654.6446479958058</v>
       </c>
       <c r="D4">
-        <v>2543.259220765488</v>
+        <v>2402.6038327594197</v>
       </c>
       <c r="E4">
-        <v>2.1427425633798518</v>
+        <v>4.2526809801803411</v>
       </c>
       <c r="F4">
-        <v>2.1427425633798509</v>
+        <v>3.3427340276185311</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -609,13 +610,13 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-4.9195194937901107E-5</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>-1.2298798734475189E-5</v>
       </c>
       <c r="K4">
-        <v>1.8929566814459612E-3</v>
+        <v>2.5093798595807594E-3</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -624,19 +625,19 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>-4.91951949379011E-5</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>-1.2298798734475145E-5</v>
       </c>
       <c r="P4">
-        <v>1.8929566814459612E-3</v>
+        <v>1.9087107441542424E-3</v>
       </c>
       <c r="Q4">
-        <v>0.51325785972267446</v>
+        <v>0.58414013555999023</v>
       </c>
       <c r="R4">
-        <v>1.9483384054563218</v>
+        <v>1.711917978451083</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -647,16 +648,16 @@
         <v>-0.4</v>
       </c>
       <c r="C5">
-        <v>4719.7359186805834</v>
+        <v>5014.9519254936731</v>
       </c>
       <c r="D5">
-        <v>2651.493623655419</v>
+        <v>2498.2889636882178</v>
       </c>
       <c r="E5">
-        <v>2.2523710459456541</v>
+        <v>4.5303576590027888</v>
       </c>
       <c r="F5">
-        <v>2.2523710459456541</v>
+        <v>3.5639702362468553</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -665,13 +666,13 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>-5.0310055972748156E-5</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>-1.2577513993187263E-5</v>
       </c>
       <c r="K5">
-        <v>1.8992564931400535E-3</v>
+        <v>2.5101163174238278E-3</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -680,19 +681,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>-5.031005597274819E-5</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>-1.2577513993187091E-5</v>
       </c>
       <c r="P5">
-        <v>1.8992564931400535E-3</v>
+        <v>1.9046321291226521E-3</v>
       </c>
       <c r="Q5">
-        <v>0.52658016506292893</v>
+        <v>0.60416191509731698</v>
       </c>
       <c r="R5">
-        <v>1.8990460832881828</v>
+        <v>1.6551854312745322</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -703,16 +704,16 @@
         <v>-0.5</v>
       </c>
       <c r="C6">
-        <v>5071.1816968796547</v>
+        <v>5401.8450121621154</v>
       </c>
       <c r="D6">
-        <v>2757.0451847163467</v>
+        <v>2590.4706060773165</v>
       </c>
       <c r="E6">
-        <v>2.378250480669732</v>
+        <v>4.854455453582343</v>
       </c>
       <c r="F6">
-        <v>2.3782504806697315</v>
+        <v>3.8226455453650194</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -721,13 +722,13 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>-5.145667790516934E-5</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>-1.2864169476292289E-5</v>
       </c>
       <c r="K6">
-        <v>1.908931149959465E-3</v>
+        <v>2.5143461243464942E-3</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -736,19 +737,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>-5.145667790516934E-5</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>-1.2864169476292518E-5</v>
       </c>
       <c r="P6">
-        <v>1.908931149959465E-3</v>
+        <v>1.9037601375470937E-3</v>
       </c>
       <c r="Q6">
-        <v>0.54128790179185893</v>
+        <v>0.62685350612646906</v>
       </c>
       <c r="R6">
-        <v>1.8474456877562531</v>
+        <v>1.5952690544547226</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -759,16 +760,16 @@
         <v>-0.6</v>
       </c>
       <c r="C7">
-        <v>5447.4477124679661</v>
+        <v>5817.5275845997367</v>
       </c>
       <c r="D7">
-        <v>2858.7037105080326</v>
+        <v>2677.9331233542935</v>
       </c>
       <c r="E7">
-        <v>2.5238772043692945</v>
+        <v>5.2361097865164723</v>
       </c>
       <c r="F7">
-        <v>2.5238772043692941</v>
+        <v>4.1278366215698696</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -777,13 +778,13 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>-5.2636152738711431E-5</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>-1.3159038184677951E-5</v>
       </c>
       <c r="K7">
-        <v>1.9220223723853268E-3</v>
+        <v>2.522037418193737E-3</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -792,19 +793,19 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>-5.2636152738711465E-5</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>-1.3159038184677914E-5</v>
       </c>
       <c r="P7">
-        <v>1.9220223723853268E-3</v>
+        <v>1.9060582344581625E-3</v>
       </c>
       <c r="Q7">
-        <v>0.55766909175255508</v>
+        <v>0.65289523691174911</v>
       </c>
       <c r="R7">
-        <v>1.7931780957365893</v>
+        <v>1.5316392944296644</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -815,16 +816,16 @@
         <v>-0.70000000000000007</v>
       </c>
       <c r="C8">
-        <v>5850.5581373992145</v>
+        <v>6264.4310235282646</v>
       </c>
       <c r="D8">
-        <v>2955.0743601967879</v>
+        <v>2759.2884620353675</v>
       </c>
       <c r="E8">
-        <v>2.6937645069250262</v>
+        <v>5.6898873681970654</v>
       </c>
       <c r="F8">
-        <v>2.6937645069250253</v>
+        <v>4.4914433120504302</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -833,13 +834,13 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>-5.3849616531832347E-5</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>-1.3462404132957992E-5</v>
       </c>
       <c r="K8">
-        <v>1.9385940445396934E-3</v>
+        <v>2.5331758847272254E-3</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -848,19 +849,19 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>-5.3849616531832259E-5</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>-1.3462404132958112E-5</v>
       </c>
       <c r="P8">
-        <v>1.9385940445396934E-3</v>
+        <v>1.9115068480491776E-3</v>
       </c>
       <c r="Q8">
-        <v>0.57609633109532643</v>
+        <v>0.68322317208738581</v>
       </c>
       <c r="R8">
-        <v>1.7358208098612771</v>
+        <v>1.46365059156995</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -871,16 +872,16 @@
         <v>-0.8</v>
       </c>
       <c r="C9">
-        <v>6282.7564837223754</v>
+        <v>6745.241859153075</v>
       </c>
       <c r="D9">
-        <v>3044.552276277625</v>
+        <v>2832.9543264556473</v>
       </c>
       <c r="E9">
-        <v>2.8938176578196089</v>
+        <v>6.234948507241719</v>
       </c>
       <c r="F9">
-        <v>2.893817657819608</v>
+        <v>4.9291576827223498</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -889,13 +890,13 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>-5.5098251440875404E-5</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>-1.3774562860218949E-5</v>
       </c>
       <c r="K9">
-        <v>1.9587328259949668E-3</v>
+        <v>2.5477641409715518E-3</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -904,19 +905,19 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>-5.5098251440875452E-5</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>-1.3774562860218961E-5</v>
       </c>
       <c r="P9">
-        <v>1.9587328259949668E-3</v>
+        <v>1.9201027464762796E-3</v>
       </c>
       <c r="Q9">
-        <v>0.59706131854692779</v>
+        <v>0.71916612461524143</v>
       </c>
       <c r="R9">
-        <v>1.6748698482656805</v>
+        <v>1.3904993099264882</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -927,16 +928,16 @@
         <v>-0.9</v>
       </c>
       <c r="C10">
-        <v>6746.5346726041216</v>
+        <v>7262.9328111705154</v>
       </c>
       <c r="D10">
-        <v>3125.2935155518803</v>
+        <v>2897.1294724868117</v>
       </c>
       <c r="E10">
-        <v>3.1318731268220041</v>
+        <v>6.8964539136457619</v>
       </c>
       <c r="F10">
-        <v>3.1318731268220033</v>
+        <v>5.4616504066088929</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -945,13 +946,13 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>-5.6383287870248444E-5</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>-1.4095821967562262E-5</v>
       </c>
       <c r="K10">
-        <v>1.982549054688879E-3</v>
+        <v>2.5658212720185893E-3</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -960,19 +961,19 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>-5.6383287870248511E-5</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>-1.4095821967562128E-5</v>
       </c>
       <c r="P10">
-        <v>1.982549054688879E-3</v>
+        <v>1.9318585656977647E-3</v>
       </c>
       <c r="Q10">
-        <v>0.62122828573975475</v>
+        <v>0.76268394774560178</v>
       </c>
       <c r="R10">
-        <v>1.6097142112729241</v>
+        <v>1.3111591019528794</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
@@ -983,16 +984,16 @@
         <v>-1</v>
       </c>
       <c r="C11">
-        <v>7244.6663923716715</v>
+        <v>7820.7979328741312</v>
       </c>
       <c r="D11">
-        <v>3195.1816910843309</v>
+        <v>2949.7657111225972</v>
       </c>
       <c r="E11">
-        <v>3.4184787990111745</v>
+        <v>7.7068738462980511</v>
       </c>
       <c r="F11">
-        <v>3.4184787990111731</v>
+        <v>6.1157135705857488</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1001,13 +1002,13 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>-5.7706006736090695E-5</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>-1.442650168402257E-5</v>
       </c>
       <c r="K11">
-        <v>2.010177956240583E-3</v>
+        <v>2.5873825051450231E-3</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1016,19 +1017,19 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>-5.770600673609077E-5</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>-1.4426501684022642E-5</v>
       </c>
       <c r="P11">
-        <v>2.010177956240583E-3</v>
+        <v>1.9468024722469435E-3</v>
       </c>
       <c r="Q11">
-        <v>0.64951990558663775</v>
+        <v>0.816808901272147</v>
       </c>
       <c r="R11">
-        <v>1.5395986965123314</v>
+        <v>1.2242765700062037</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
@@ -1039,16 +1040,16 @@
         <v>-1.1000000000000001</v>
       </c>
       <c r="C12">
-        <v>7780.2454373356604</v>
+        <v>8422.4924480112459</v>
       </c>
       <c r="D12">
-        <v>3251.7896333803437</v>
+        <v>2988.5361498564334</v>
       </c>
       <c r="E12">
-        <v>3.7680184732992452</v>
+        <v>8.7058865668479015</v>
       </c>
       <c r="F12">
-        <v>3.7680184732992439</v>
+        <v>6.9243296968215331</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1057,13 +1058,13 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>-5.9067741850124972E-5</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>-1.4766935462531348E-5</v>
       </c>
       <c r="K12">
-        <v>2.0417811813262981E-3</v>
+        <v>2.6124990064920711E-3</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1072,19 +1073,19 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>-5.9067741850124918E-5</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>-1.4766935462531335E-5</v>
       </c>
       <c r="P12">
-        <v>2.0417811813262981E-3</v>
+        <v>1.9649779462084498E-3</v>
       </c>
       <c r="Q12">
-        <v>0.68326190202175985</v>
+        <v>0.88653102777918047</v>
       </c>
       <c r="R12">
-        <v>1.4635676261782162</v>
+        <v>1.1279921048054764</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
@@ -1095,16 +1096,16 @@
         <v>-1.2000000000000002</v>
       </c>
       <c r="C13">
-        <v>8356.7298410593485</v>
+        <v>9072.0779618754823</v>
       </c>
       <c r="D13">
-        <v>3292.3352571166524</v>
+        <v>3010.7991262202277</v>
       </c>
       <c r="E13">
-        <v>4.2002880280494566</v>
+        <v>9.9347804799948989</v>
       </c>
       <c r="F13">
-        <v>4.2002880280494583</v>
+        <v>7.9224323678235313</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1113,13 +1114,13 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>-6.0469882430826394E-5</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>-1.511747060770676E-5</v>
       </c>
       <c r="K13">
-        <v>2.0775486997065343E-3</v>
+        <v>2.6412377863381463E-3</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1128,19 +1129,19 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>-6.0469882430826428E-5</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>-1.5117470607706607E-5</v>
       </c>
       <c r="P13">
-        <v>2.0775486997065343E-3</v>
+        <v>1.9864436704326869E-3</v>
       </c>
       <c r="Q13">
-        <v>0.72444048147314899</v>
+        <v>0.98077036243025495</v>
       </c>
       <c r="R13">
-        <v>1.3803756493100732</v>
+        <v>1.0196066666636376</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
@@ -1151,16 +1152,16 @@
         <v>-1.3000000000000003</v>
       </c>
       <c r="C14">
-        <v>8977.9927630715356</v>
+        <v>9774.0738372021879</v>
       </c>
       <c r="D14">
-        <v>3313.6306744284634</v>
+        <v>3013.5572017344052</v>
       </c>
       <c r="E14">
-        <v>4.7425101144814406</v>
+        <v>11.414391132797533</v>
       </c>
       <c r="F14">
-        <v>4.7425101144814397</v>
+        <v>9.1296590311547909</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1169,13 +1170,13 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>-6.191387574950792E-5</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>-1.5478468937377034E-5</v>
       </c>
       <c r="K14">
-        <v>2.1177010872130784E-3</v>
+        <v>2.6736816991370666E-3</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1184,19 +1185,19 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>-6.1913875749507947E-5</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>-1.5478468937377153E-5</v>
       </c>
       <c r="P14">
-        <v>2.1177010872130784E-3</v>
+        <v>2.0112735121486777E-3</v>
       </c>
       <c r="Q14">
-        <v>0.77619381406565968</v>
+        <v>1.117454321393577</v>
       </c>
       <c r="R14">
-        <v>1.2883380180035913</v>
+        <v>0.89489116544191294</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
@@ -1207,16 +1208,16 @@
         <v>-1.4000000000000001</v>
       </c>
       <c r="C15">
-        <v>9648.3812616691957</v>
+        <v>10533.515653927709</v>
       </c>
       <c r="D15">
-        <v>3312.0234221068076</v>
+        <v>2993.4104834709942</v>
       </c>
       <c r="E15">
-        <v>5.4311565622915756</v>
+        <v>13.083928524060575</v>
       </c>
       <c r="F15">
-        <v>5.4311565622915774</v>
+        <v>10.502255888113682</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1225,13 +1226,13 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>-6.3401229919424521E-5</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>-1.5850307479856073E-5</v>
       </c>
       <c r="K15">
-        <v>2.1624922507450955E-3</v>
+        <v>2.709929523936274E-3</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1240,19 +1241,467 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>-6.3401229919424657E-5</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>-1.5850307479856107E-5</v>
       </c>
       <c r="P15">
-        <v>2.1624922507450955E-3</v>
+        <v>2.0395565825618812E-3</v>
       </c>
       <c r="Q15">
-        <v>0.84383898207024499</v>
+        <v>1.3397443477165478</v>
       </c>
       <c r="R15">
-        <v>1.1850602084613762</v>
+        <v>0.74641106096427579</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="B16">
+        <v>-1.5000000000000002</v>
+      </c>
+      <c r="C16">
+        <v>11356.021823632545</v>
+      </c>
+      <c r="D16">
+        <v>2946.503421598944</v>
+      </c>
+      <c r="E16">
+        <v>14.684966376713492</v>
+      </c>
+      <c r="F16">
+        <v>11.842983718706254</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>-6.4933516836537594E-5</v>
+      </c>
+      <c r="J16">
+        <v>-1.6233379209134514E-5</v>
+      </c>
+      <c r="K16">
+        <v>2.7500961094330824E-3</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>-6.493351683653754E-5</v>
+      </c>
+      <c r="O16">
+        <v>-1.6233379209134155E-5</v>
+      </c>
+      <c r="P16">
+        <v>2.0713973586521579E-3</v>
+      </c>
+      <c r="Q16">
+        <v>1.7912550861998784</v>
+      </c>
+      <c r="R16">
+        <v>0.55826777978422126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1.6</v>
+      </c>
+      <c r="B17">
+        <v>-1.6</v>
+      </c>
+      <c r="C17">
+        <v>12247.869609212974</v>
+      </c>
+      <c r="D17">
+        <v>2868.4640912095715</v>
+      </c>
+      <c r="E17">
+        <v>15.69566566961147</v>
+      </c>
+      <c r="F17">
+        <v>12.768417751247265</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>-6.6512375281157891E-5</v>
+      </c>
+      <c r="J17">
+        <v>-1.6628093820289415E-5</v>
+      </c>
+      <c r="K17">
+        <v>2.7943125656287727E-3</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>-6.6512375281158393E-5</v>
+      </c>
+      <c r="O17">
+        <v>-1.6628093820289717E-5</v>
+      </c>
+      <c r="P17">
+        <v>2.10691584907398E-3</v>
+      </c>
+      <c r="Q17">
+        <v>3.606090610469928</v>
+      </c>
+      <c r="R17">
+        <v>0.27730861700940035</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="B18">
+        <v>-1.7000000000000002</v>
+      </c>
+      <c r="C18">
+        <v>13216.08201377174</v>
+      </c>
+      <c r="D18">
+        <v>2754.3348012184429</v>
+      </c>
+      <c r="E18">
+        <v>15.627632693193997</v>
+      </c>
+      <c r="F18">
+        <v>13.209996628822301</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>-6.8139514190305127E-5</v>
+      </c>
+      <c r="J18">
+        <v>-1.7034878547576221E-5</v>
+      </c>
+      <c r="K18">
+        <v>2.8427264806007752E-3</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>-6.8139514190305195E-5</v>
+      </c>
+      <c r="O18">
+        <v>-1.7034878547576299E-5</v>
+      </c>
+      <c r="P18">
+        <v>2.1462477826069367E-3</v>
+      </c>
+      <c r="Q18">
+        <v>8.0000000000000036</v>
+      </c>
+      <c r="R18">
+        <v>-0.12499999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1.8000000000000003</v>
+      </c>
+      <c r="B19">
+        <v>-1.8000000000000003</v>
+      </c>
+      <c r="C19">
+        <v>14268.527256958694</v>
+      </c>
+      <c r="D19">
+        <v>2598.4926771113714</v>
+      </c>
+      <c r="E19">
+        <v>14.578801077706167</v>
+      </c>
+      <c r="F19">
+        <v>12.656981686379355</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>-6.9816716111289554E-5</v>
+      </c>
+      <c r="J19">
+        <v>-1.7454179027822449E-5</v>
+      </c>
+      <c r="K19">
+        <v>2.8955021360626359E-3</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>-6.981671611128954E-5</v>
+      </c>
+      <c r="O19">
+        <v>-1.7454179027822571E-5</v>
+      </c>
+      <c r="P19">
+        <v>2.1895447927393406E-3</v>
+      </c>
+      <c r="Q19">
+        <v>8.0000000000000107</v>
+      </c>
+      <c r="R19">
+        <v>-0.12499999999999983</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1.9000000000000001</v>
+      </c>
+      <c r="B20">
+        <v>-1.9000000000000001</v>
+      </c>
+      <c r="C20">
+        <v>15414.032860746493</v>
+      </c>
+      <c r="D20">
+        <v>2394.5586315304267</v>
+      </c>
+      <c r="E20">
+        <v>13.106170090370204</v>
+      </c>
+      <c r="F20">
+        <v>11.211026461110826</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>-7.1545840847735224E-5</v>
+      </c>
+      <c r="J20">
+        <v>-1.7886460211933806E-5</v>
+      </c>
+      <c r="K20">
+        <v>2.9528206887606693E-3</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>-7.1545840847735197E-5</v>
+      </c>
+      <c r="O20">
+        <v>-1.7886460211933864E-5</v>
+      </c>
+      <c r="P20">
+        <v>2.236974565332151E-3</v>
+      </c>
+      <c r="Q20">
+        <v>8</v>
+      </c>
+      <c r="R20">
+        <v>-0.125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>-2</v>
+      </c>
+      <c r="C21">
+        <v>16662.516730687603</v>
+      </c>
+      <c r="D21">
+        <v>2135.2928595825151</v>
+      </c>
+      <c r="E21">
+        <v>11.63792304657953</v>
+      </c>
+      <c r="F21">
+        <v>9.8584694850896213</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>-7.332882931003407E-5</v>
+      </c>
+      <c r="J21">
+        <v>-1.8332207327508453E-5</v>
+      </c>
+      <c r="K21">
+        <v>3.0148802758904283E-3</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>-7.332882931003426E-5</v>
+      </c>
+      <c r="O21">
+        <v>-1.8332207327508565E-5</v>
+      </c>
+      <c r="P21">
+        <v>2.2887209074297274E-3</v>
+      </c>
+      <c r="Q21">
+        <v>7.9999999999999964</v>
+      </c>
+      <c r="R21">
+        <v>-0.12500000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2.1</v>
+      </c>
+      <c r="B22">
+        <v>-2.1</v>
+      </c>
+      <c r="C22">
+        <v>18025.138056472686</v>
+      </c>
+      <c r="D22">
+        <v>1812.4746649874137</v>
+      </c>
+      <c r="E22">
+        <v>10.358828073365133</v>
+      </c>
+      <c r="F22">
+        <v>8.8329017791809488</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>-7.516770758304521E-5</v>
+      </c>
+      <c r="J22">
+        <v>-1.8791926895761302E-5</v>
+      </c>
+      <c r="K22">
+        <v>3.0818959909812557E-3</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>-7.5167707583045359E-5</v>
+      </c>
+      <c r="O22">
+        <v>-1.879192689576154E-5</v>
+      </c>
+      <c r="P22">
+        <v>2.3449836835334119E-3</v>
+      </c>
+      <c r="Q22">
+        <v>8</v>
+      </c>
+      <c r="R22">
+        <v>-0.125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B23">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="C23">
+        <v>19514.47138381589</v>
+      </c>
+      <c r="D23">
+        <v>1416.7640273239806</v>
+      </c>
+      <c r="E23">
+        <v>9.3077870157774782</v>
+      </c>
+      <c r="F23">
+        <v>8.0211324992448176</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>-7.7064591224747537E-5</v>
+      </c>
+      <c r="J23">
+        <v>-1.9266147806186678E-5</v>
+      </c>
+      <c r="K23">
+        <v>3.1540996612727185E-3</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>-7.706459122474747E-5</v>
+      </c>
+      <c r="O23">
+        <v>-1.9266147806186935E-5</v>
+      </c>
+      <c r="P23">
+        <v>2.4059785502134777E-3</v>
+      </c>
+      <c r="Q23">
+        <v>8.0000000000000071</v>
+      </c>
+      <c r="R23">
+        <v>-0.12499999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>